<commit_message>
Updated gitgnore and Excel for mapping
</commit_message>
<xml_diff>
--- a/Create_MappingXml_File.xlsx
+++ b/Create_MappingXml_File.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ralf/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ralf/Documents/GitHub/LocDbConverterConsole/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE6733E-365A-834A-9E65-76E3240FDFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF678707-46E0-724B-8B09-CCA6E9208CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2020" yWindow="3520" windowWidth="35940" windowHeight="20780" xr2:uid="{DA64CF93-7AD7-5549-BC85-4B8B89C6C2C1}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="z21" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$H$234</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$F$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1246,16 +1246,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1582,7 +1587,7 @@
   <dimension ref="A1:H235"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1592,24 +1597,24 @@
     <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="45.6640625" customWidth="1"/>
-    <col min="8" max="8" width="92" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="92" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="H1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="H1" s="8" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F2" s="1"/>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="8" t="s">
         <v>329</v>
       </c>
     </row>
@@ -1632,7 +1637,7 @@
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="8" t="s">
         <v>331</v>
       </c>
     </row>
@@ -1653,10 +1658,10 @@
       <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="H4" s="5" t="str">
+      <c r="H4" s="8" t="str">
         <f>"&lt;mapping Id="""&amp;A4&amp;""" Shortname="""&amp;B4&amp;""" Duration="""&amp;C4&amp;""" FunctionTypeCS2="""&amp;E4&amp;""" FunctionTypeZ21="""&amp;F4&amp;""" /&gt;"</f>
         <v>&lt;mapping Id="1" Shortname="Lchtwchsl" Duration="0" FunctionTypeCS2="Lichtwechsel" FunctionTypeZ21="main_beam2" /&gt;</v>
       </c>
@@ -1678,10 +1683,10 @@
       <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="H5" s="5" t="str">
+      <c r="H5" s="8" t="str">
         <f t="shared" ref="H5:H68" si="1">"&lt;mapping Id="""&amp;A5&amp;""" Shortname="""&amp;B5&amp;""" Duration="""&amp;C5&amp;""" FunctionTypeCS2="""&amp;E5&amp;""" FunctionTypeZ21="""&amp;F5&amp;""" /&gt;"</f>
         <v>&lt;mapping Id="2" Shortname="Innnblchtn" Duration="0" FunctionTypeCS2="Innenbeleuchtung" FunctionTypeZ21="interior_light" /&gt;</v>
       </c>
@@ -1703,10 +1708,10 @@
       <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="H6" s="5" t="str">
+      <c r="H6" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="3" Shortname="Assnblchtn" Duration="0" FunctionTypeCS2="Aussenbeleuchtung_Schlusslicht" FunctionTypeZ21="back_light" /&gt;</v>
       </c>
@@ -1728,10 +1733,10 @@
       <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="H7" s="5" t="str">
+      <c r="H7" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="4" Shortname="Fernlicht" Duration="0" FunctionTypeCS2="Fernlicht" FunctionTypeZ21="main_beam" /&gt;</v>
       </c>
@@ -1753,10 +1758,10 @@
       <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="5" t="str">
+      <c r="H8" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="5" Shortname="Btrbsgrsch" Duration="0" FunctionTypeCS2="Betriebsgeraeusch" FunctionTypeZ21="sound2" /&gt;</v>
       </c>
@@ -1778,10 +1783,10 @@
       <c r="E9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="H9" s="5" t="str">
+      <c r="H9" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="6" Shortname="Pantograph" Duration="0" FunctionTypeCS2="Pantograph" FunctionTypeZ21="backward_take_power" /&gt;</v>
       </c>
@@ -1803,10 +1808,10 @@
       <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="5" t="str">
+      <c r="H10" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="7" Shortname="Rchgnrtr" Duration="0" FunctionTypeCS2="Rauchgenerator" FunctionTypeZ21="steam" /&gt;</v>
       </c>
@@ -1828,10 +1833,10 @@
       <c r="E11" t="s">
         <v>18</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="5" t="str">
+      <c r="H11" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="8" Shortname="Rngrgng_n" Duration="0" FunctionTypeCS2="Rangiergang_ein" FunctionTypeZ21="hump_gear" /&gt;</v>
       </c>
@@ -1853,10 +1858,10 @@
       <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="H12" s="5" t="str">
+      <c r="H12" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="9" Shortname="Tlxkpplng" Duration="0" FunctionTypeCS2="Telexkupplung" FunctionTypeZ21="decouple" /&gt;</v>
       </c>
@@ -1878,10 +1883,10 @@
       <c r="E13" t="s">
         <v>20</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="H13" s="5" t="str">
+      <c r="H13" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="10" Shortname="Hrn_Typhn" Duration="0" FunctionTypeCS2="Horn_Typhon" FunctionTypeZ21="bugle" /&gt;</v>
       </c>
@@ -1903,10 +1908,10 @@
       <c r="E14" t="s">
         <v>21</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="H14" s="5" t="str">
+      <c r="H14" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="11" Shortname="Schffnrpff" Duration="0" FunctionTypeCS2="Schaffnerpfiff" FunctionTypeZ21="sound5" /&gt;</v>
       </c>
@@ -1928,10 +1933,10 @@
       <c r="E15" t="s">
         <v>22</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="H15" s="5" t="str">
+      <c r="H15" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="12" Shortname="Pfeife" Duration="0" FunctionTypeCS2="Pfeife" FunctionTypeZ21="sound4" /&gt;</v>
       </c>
@@ -1953,10 +1958,10 @@
       <c r="E16" t="s">
         <v>23</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="H16" s="5" t="str">
+      <c r="H16" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="13" Shortname="Glocke" Duration="0" FunctionTypeCS2="Glocke" FunctionTypeZ21="bell" /&gt;</v>
       </c>
@@ -1978,7 +1983,8 @@
       <c r="E17" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="5" t="str">
+      <c r="F17" s="7"/>
+      <c r="H17" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="14" Shortname="KrnBhn_vrf" Duration="0" FunctionTypeCS2="KranBuehne_verfahren" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -2000,7 +2006,8 @@
       <c r="E18" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="5" t="str">
+      <c r="F18" s="7"/>
+      <c r="H18" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="15" Shortname="KrnBhn_hbn" Duration="0" FunctionTypeCS2="KranBuehne_heben_senken" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -2022,7 +2029,8 @@
       <c r="E19" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="5" t="str">
+      <c r="F19" s="7"/>
+      <c r="H19" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="16" Shortname="KrnBhn_drh" Duration="0" FunctionTypeCS2="KranBuehne_drehen_links" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -2044,7 +2052,8 @@
       <c r="E20" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="5" t="str">
+      <c r="F20" s="7"/>
+      <c r="H20" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="17" Shortname="KrnBhn_ngn" Duration="0" FunctionTypeCS2="KranBuehne_neigen" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -2066,10 +2075,10 @@
       <c r="E21" t="s">
         <v>28</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="H21" s="5" t="str">
+      <c r="H21" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="18" Shortname="Anfhr_Brms" Duration="0" FunctionTypeCS2="Anfahr_Bremsverzoegerung_aus" FunctionTypeZ21="acc_delay" /&gt;</v>
       </c>
@@ -2091,10 +2100,10 @@
       <c r="E22" t="s">
         <v>29</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="H22" s="5" t="str">
+      <c r="H22" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="19" Shortname="Pumpe" Duration="0" FunctionTypeCS2="Pumpe" FunctionTypeZ21="feed_pump" /&gt;</v>
       </c>
@@ -2116,10 +2125,10 @@
       <c r="E23" t="s">
         <v>30</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="H23" s="5" t="str">
+      <c r="H23" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="20" Shortname="Brmsnqtsch" Duration="0" FunctionTypeCS2="Bremsenquietschen_aus" FunctionTypeZ21="sound_brake" /&gt;</v>
       </c>
@@ -2141,10 +2150,10 @@
       <c r="E24" t="s">
         <v>31</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="H24" s="5" t="str">
+      <c r="H24" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="21" Shortname="Schltstfn" Duration="0" FunctionTypeCS2="Schaltstufen" FunctionTypeZ21="diesel_regulation_step_up" /&gt;</v>
       </c>
@@ -2166,10 +2175,10 @@
       <c r="E25" t="s">
         <v>32</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="H25" s="5" t="str">
+      <c r="H25" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="22" Shortname="Generator" Duration="0" FunctionTypeCS2="Generator" FunctionTypeZ21="generator" /&gt;</v>
       </c>
@@ -2191,10 +2200,10 @@
       <c r="E26" t="s">
         <v>33</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="5" t="str">
+      <c r="H26" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="23" Shortname="Fhrgrsch" Duration="0" FunctionTypeCS2="Fahrgeraeusch" FunctionTypeZ21="sound2" /&gt;</v>
       </c>
@@ -2216,7 +2225,8 @@
       <c r="E27" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="5" t="str">
+      <c r="F27" s="7"/>
+      <c r="H27" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="24" Shortname="Mschn_vrsc" Duration="0" FunctionTypeCS2="Maschine_vorschmieren" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -2238,10 +2248,10 @@
       <c r="E28" t="s">
         <v>35</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="H28" s="5" t="str">
+      <c r="H28" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="25" Shortname="Bhnhfsnsg" Duration="0" FunctionTypeCS2="Bahnhofsansage" FunctionTypeZ21="sound1" /&gt;</v>
       </c>
@@ -2263,10 +2273,10 @@
       <c r="E29" t="s">
         <v>36</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="H29" s="5" t="str">
+      <c r="H29" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="26" Shortname="Khln_schfl" Duration="0" FunctionTypeCS2="Kohlen_schaufeln" FunctionTypeZ21="scoop_coal" /&gt;</v>
       </c>
@@ -2288,7 +2298,8 @@
       <c r="E30" t="s">
         <v>37</v>
       </c>
-      <c r="H30" s="5" t="str">
+      <c r="F30" s="7"/>
+      <c r="H30" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="27" Shortname="Trn_schlss" Duration="0" FunctionTypeCS2="Tueren_schliessen" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -2310,10 +2321,10 @@
       <c r="E31" t="s">
         <v>38</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="H31" s="5" t="str">
+      <c r="H31" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="28" Shortname="Trn_schlss" Duration="0" FunctionTypeCS2="Tueren_schliessen_Geraeusch" FunctionTypeZ21="door_close" /&gt;</v>
       </c>
@@ -2335,10 +2346,10 @@
       <c r="E32" t="s">
         <v>39</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="H32" s="5" t="str">
+      <c r="H32" s="8" t="str">
         <f>"&lt;mapping Id="""&amp;A32&amp;""" Shortname="""&amp;B32&amp;""" Duration="""&amp;C32&amp;""" FunctionTypeCS2="""&amp;E32&amp;""" FunctionTypeZ21="""&amp;F32&amp;""" /&gt;"</f>
         <v>&lt;mapping Id="29" Shortname="Lftrgrsch" Duration="0" FunctionTypeCS2="Lueftergeraeusch" FunctionTypeZ21="sound4" /&gt;</v>
       </c>
@@ -2360,7 +2371,8 @@
       <c r="E33" t="s">
         <v>40</v>
       </c>
-      <c r="H33" s="5" t="str">
+      <c r="F33" s="7"/>
+      <c r="H33" s="8" t="str">
         <f>"&lt;mapping Id="""&amp;A33&amp;""" Shortname="""&amp;B33&amp;""" Duration="""&amp;C33&amp;""" FunctionTypeCS2="""&amp;E33&amp;""" FunctionTypeZ21="""&amp;F33&amp;""" /&gt;"</f>
         <v>&lt;mapping Id="30" Shortname="Luefter" Duration="0" FunctionTypeCS2="Luefter" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -2382,7 +2394,8 @@
       <c r="E34" t="s">
         <v>41</v>
       </c>
-      <c r="H34" s="5" t="str">
+      <c r="F34" s="7"/>
+      <c r="H34" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="31" Shortname="Frbchsnblc" Duration="0" FunctionTypeCS2="Feuerbuechsenbeleuchtung" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -2404,10 +2417,10 @@
       <c r="E35" t="s">
         <v>42</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="H35" s="5" t="str">
+      <c r="H35" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="32" Shortname="Dcknblchtn" Duration="0" FunctionTypeCS2="Deckenbeleuchtung" FunctionTypeZ21="interior_light" /&gt;</v>
       </c>
@@ -2429,10 +2442,10 @@
       <c r="E36" t="s">
         <v>43</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="H36" s="5" t="str">
+      <c r="H36" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="33" Shortname="Tschblchtn" Duration="0" FunctionTypeCS2="Tischbeleuchtung_EP4" FunctionTypeZ21="tish_lamp" /&gt;</v>
       </c>
@@ -2454,10 +2467,10 @@
       <c r="E37" t="s">
         <v>44</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="H37" s="5" t="str">
+      <c r="H37" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="34" Shortname="Tschblchtn" Duration="0" FunctionTypeCS2="Tischbeleuchtung_EP3" FunctionTypeZ21="tish_lamp" /&gt;</v>
       </c>
@@ -2479,10 +2492,10 @@
       <c r="E38" t="s">
         <v>45</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="H38" s="5" t="str">
+      <c r="H38" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="35" Shortname="Tschblchtn" Duration="0" FunctionTypeCS2="Tischbeleuchtung_EP2" FunctionTypeZ21="tish_lamp" /&gt;</v>
       </c>
@@ -2504,10 +2517,10 @@
       <c r="E39" t="s">
         <v>46</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="H39" s="5" t="str">
+      <c r="H39" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="36" Shortname="Schttlrst" Duration="0" FunctionTypeCS2="Schuettelrost" FunctionTypeZ21="shaking_grates" /&gt;</v>
       </c>
@@ -2529,10 +2542,10 @@
       <c r="E40" t="s">
         <v>333</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="H40" s="5" t="str">
+      <c r="H40" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="37" Shortname="Schnnstss" Duration="0" FunctionTypeCS2="Schienenstoss" FunctionTypeZ21="rail_kick" /&gt;</v>
       </c>
@@ -2554,10 +2567,10 @@
       <c r="E41" t="s">
         <v>47</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="H41" s="5" t="str">
+      <c r="H41" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="38" Shortname="Nmmrnschld" Duration="0" FunctionTypeCS2="Nummernschildbeleuchtung" FunctionTypeZ21="licence_plate_light" /&gt;</v>
       </c>
@@ -2579,10 +2592,10 @@
       <c r="E42" t="s">
         <v>48</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="H42" s="5" t="str">
+      <c r="H42" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="39" Shortname="Hntrgrndms" Duration="0" FunctionTypeCS2="Hintergrundmusik" FunctionTypeZ21="clef" /&gt;</v>
       </c>
@@ -2604,10 +2617,10 @@
       <c r="E43" t="s">
         <v>49</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="H43" s="5" t="str">
+      <c r="H43" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="40" Shortname="Zglfschldb" Duration="0" FunctionTypeCS2="Zuglaufschildbeleuchtung" FunctionTypeZ21="destination_plate_light" /&gt;</v>
       </c>
@@ -2629,10 +2642,10 @@
       <c r="E44" t="s">
         <v>50</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="H44" s="5" t="str">
+      <c r="H44" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="41" Shortname="Lcht_n_Fhr" Duration="0" FunctionTypeCS2="Licht_an_Fuehrerstand_hinten_aus" FunctionTypeZ21="cockpit_light_right" /&gt;</v>
       </c>
@@ -2654,10 +2667,10 @@
       <c r="E45" t="s">
         <v>51</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="H45" s="5" t="str">
+      <c r="H45" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="42" Shortname="Lcht_n_Fhr" Duration="0" FunctionTypeCS2="Licht_an_Fuehrerstand_vorne_aus" FunctionTypeZ21="cockpit_light_left" /&gt;</v>
       </c>
@@ -2679,10 +2692,10 @@
       <c r="E46" t="s">
         <v>52</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="H46" s="5" t="str">
+      <c r="H46" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="43" Shortname="Kpplng_An_" Duration="0" FunctionTypeCS2="Kupplung_An_Abkuppelgeraeusch" FunctionTypeZ21="decouple" /&gt;</v>
       </c>
@@ -2704,10 +2717,10 @@
       <c r="E47" t="s">
         <v>53</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="H47" s="5" t="str">
+      <c r="H47" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="44" Shortname="Pffrstss" Duration="0" FunctionTypeCS2="Pufferstoss" FunctionTypeZ21="puffer_kick" /&gt;</v>
       </c>
@@ -2729,10 +2742,10 @@
       <c r="E48" t="s">
         <v>54</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H48" s="5" t="str">
+      <c r="H48" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="45" Shortname="Sprchsgb" Duration="0" FunctionTypeCS2="Sprachausgabe" FunctionTypeZ21="sound2" /&gt;</v>
       </c>
@@ -2754,7 +2767,8 @@
       <c r="E49" t="s">
         <v>55</v>
       </c>
-      <c r="H49" s="5" t="str">
+      <c r="F49" s="7"/>
+      <c r="H49" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="46" Shortname="Krn_Dpplhk" Duration="0" FunctionTypeCS2="Kran_Doppelhaken" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -2776,10 +2790,10 @@
       <c r="E50" t="s">
         <v>56</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="H50" s="5" t="str">
+      <c r="H50" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="47" Shortname="Warnlicht" Duration="0" FunctionTypeCS2="Warnlicht" FunctionTypeZ21="all_round_light" /&gt;</v>
       </c>
@@ -2801,10 +2815,10 @@
       <c r="E51" t="s">
         <v>57</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="H51" s="5" t="str">
+      <c r="H51" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="48" Shortname="Fhrrstndsb" Duration="0" FunctionTypeCS2="Fuehrerstandsbeleuchtung" FunctionTypeZ21="cockpit_light_left" /&gt;</v>
       </c>
@@ -2826,10 +2840,10 @@
       <c r="E52" t="s">
         <v>58</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="H52" s="5" t="str">
+      <c r="H52" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="49" Shortname="Injektor" Duration="0" FunctionTypeCS2="Injektor" FunctionTypeZ21="injector" /&gt;</v>
       </c>
@@ -2851,10 +2865,10 @@
       <c r="E53" t="s">
         <v>59</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H53" s="5" t="str">
+      <c r="H53" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="50" Shortname="Funktion_0" Duration="0" FunctionTypeCS2="Funktion_0" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -2876,10 +2890,10 @@
       <c r="E54" t="s">
         <v>60</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H54" s="5" t="str">
+      <c r="H54" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="51" Shortname="Funktion_1" Duration="0" FunctionTypeCS2="Funktion_1" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -2901,10 +2915,10 @@
       <c r="E55" t="s">
         <v>61</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H55" s="5" t="str">
+      <c r="H55" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="52" Shortname="Funktion_2" Duration="0" FunctionTypeCS2="Funktion_2" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -2926,10 +2940,10 @@
       <c r="E56" t="s">
         <v>62</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H56" s="5" t="str">
+      <c r="H56" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="53" Shortname="Funktion_3" Duration="0" FunctionTypeCS2="Funktion_3" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -2951,10 +2965,10 @@
       <c r="E57" t="s">
         <v>63</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H57" s="5" t="str">
+      <c r="H57" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="54" Shortname="Funktion_4" Duration="0" FunctionTypeCS2="Funktion_4" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -2976,10 +2990,10 @@
       <c r="E58" t="s">
         <v>64</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H58" s="5" t="str">
+      <c r="H58" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="55" Shortname="Funktion_5" Duration="0" FunctionTypeCS2="Funktion_5" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3001,10 +3015,10 @@
       <c r="E59" t="s">
         <v>65</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H59" s="5" t="str">
+      <c r="H59" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="56" Shortname="Funktion_6" Duration="0" FunctionTypeCS2="Funktion_6" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3026,10 +3040,10 @@
       <c r="E60" t="s">
         <v>66</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H60" s="5" t="str">
+      <c r="H60" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="57" Shortname="Funktion_7" Duration="0" FunctionTypeCS2="Funktion_7" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3051,10 +3065,10 @@
       <c r="E61" t="s">
         <v>67</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H61" s="5" t="str">
+      <c r="H61" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="58" Shortname="Funktion_8" Duration="0" FunctionTypeCS2="Funktion_8" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3076,10 +3090,10 @@
       <c r="E62" t="s">
         <v>68</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H62" s="5" t="str">
+      <c r="H62" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="59" Shortname="Funktion_9" Duration="0" FunctionTypeCS2="Funktion_9" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3101,10 +3115,10 @@
       <c r="E63" t="s">
         <v>69</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H63" s="5" t="str">
+      <c r="H63" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="60" Shortname="Fnktn_10" Duration="0" FunctionTypeCS2="Funktion_10" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3126,10 +3140,10 @@
       <c r="E64" t="s">
         <v>70</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H64" s="5" t="str">
+      <c r="H64" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="61" Shortname="Fnktn_11" Duration="0" FunctionTypeCS2="Funktion_11" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3151,10 +3165,10 @@
       <c r="E65" t="s">
         <v>71</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H65" s="5" t="str">
+      <c r="H65" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="62" Shortname="Fnktn_12" Duration="0" FunctionTypeCS2="Funktion_12" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3176,10 +3190,10 @@
       <c r="E66" t="s">
         <v>72</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H66" s="5" t="str">
+      <c r="H66" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="63" Shortname="Fnktn_13" Duration="0" FunctionTypeCS2="Funktion_13" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3201,10 +3215,10 @@
       <c r="E67" t="s">
         <v>73</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H67" s="5" t="str">
+      <c r="H67" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="64" Shortname="Fnktn_14" Duration="0" FunctionTypeCS2="Funktion_14" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3226,10 +3240,10 @@
       <c r="E68" t="s">
         <v>74</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H68" s="5" t="str">
+      <c r="H68" s="8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;mapping Id="65" Shortname="Fnktn_15" Duration="0" FunctionTypeCS2="Funktion_15" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3251,10 +3265,10 @@
       <c r="E69" t="s">
         <v>75</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H69" s="5" t="str">
+      <c r="H69" s="8" t="str">
         <f t="shared" ref="H69:H132" si="3">"&lt;mapping Id="""&amp;A69&amp;""" Shortname="""&amp;B69&amp;""" Duration="""&amp;C69&amp;""" FunctionTypeCS2="""&amp;E69&amp;""" FunctionTypeZ21="""&amp;F69&amp;""" /&gt;"</f>
         <v>&lt;mapping Id="66" Shortname="Fnktn_16" Duration="0" FunctionTypeCS2="Funktion_16" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3276,10 +3290,10 @@
       <c r="E70" t="s">
         <v>76</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H70" s="5" t="str">
+      <c r="H70" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="67" Shortname="Fnktn_17" Duration="0" FunctionTypeCS2="Funktion_17" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3301,10 +3315,10 @@
       <c r="E71" t="s">
         <v>77</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H71" s="5" t="str">
+      <c r="H71" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="68" Shortname="Fnktn_18" Duration="0" FunctionTypeCS2="Funktion_18" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3326,10 +3340,10 @@
       <c r="E72" t="s">
         <v>78</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H72" s="5" t="str">
+      <c r="H72" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="69" Shortname="Fnktn_19" Duration="0" FunctionTypeCS2="Funktion_19" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3351,10 +3365,10 @@
       <c r="E73" t="s">
         <v>79</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H73" s="5" t="str">
+      <c r="H73" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="70" Shortname="Fnktn_20" Duration="0" FunctionTypeCS2="Funktion_20" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3376,10 +3390,10 @@
       <c r="E74" t="s">
         <v>80</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H74" s="5" t="str">
+      <c r="H74" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="71" Shortname="Fnktn_21" Duration="0" FunctionTypeCS2="Funktion_21" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3401,10 +3415,10 @@
       <c r="E75" t="s">
         <v>81</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H75" s="5" t="str">
+      <c r="H75" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="72" Shortname="Fnktn_22" Duration="0" FunctionTypeCS2="Funktion_22" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3426,10 +3440,10 @@
       <c r="E76" t="s">
         <v>82</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H76" s="5" t="str">
+      <c r="H76" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="73" Shortname="Fnktn_23" Duration="0" FunctionTypeCS2="Funktion_23" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3451,10 +3465,10 @@
       <c r="E77" t="s">
         <v>83</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H77" s="5" t="str">
+      <c r="H77" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="74" Shortname="Fnktn_24" Duration="0" FunctionTypeCS2="Funktion_24" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3476,10 +3490,10 @@
       <c r="E78" t="s">
         <v>84</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H78" s="5" t="str">
+      <c r="H78" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="75" Shortname="Fnktn_25" Duration="0" FunctionTypeCS2="Funktion_25" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3501,10 +3515,10 @@
       <c r="E79" t="s">
         <v>85</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H79" s="5" t="str">
+      <c r="H79" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="76" Shortname="Fnktn_26" Duration="0" FunctionTypeCS2="Funktion_26" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3526,10 +3540,10 @@
       <c r="E80" t="s">
         <v>86</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H80" s="5" t="str">
+      <c r="H80" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="77" Shortname="Fnktn_27" Duration="0" FunctionTypeCS2="Funktion_27" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3551,10 +3565,10 @@
       <c r="E81" t="s">
         <v>87</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H81" s="5" t="str">
+      <c r="H81" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="78" Shortname="Fnktn_28" Duration="0" FunctionTypeCS2="Funktion_28" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3576,10 +3590,10 @@
       <c r="E82" t="s">
         <v>88</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H82" s="5" t="str">
+      <c r="H82" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="79" Shortname="Fnktn_29" Duration="0" FunctionTypeCS2="Funktion_29" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3601,10 +3615,10 @@
       <c r="E83" t="s">
         <v>89</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H83" s="5" t="str">
+      <c r="H83" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="80" Shortname="Fnktn_30" Duration="0" FunctionTypeCS2="Funktion_30" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3626,10 +3640,10 @@
       <c r="E84" t="s">
         <v>90</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H84" s="5" t="str">
+      <c r="H84" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="81" Shortname="Fnktn_31" Duration="0" FunctionTypeCS2="Funktion_31" FunctionTypeZ21="neutral" /&gt;</v>
       </c>
@@ -3651,10 +3665,10 @@
       <c r="E85" t="s">
         <v>91</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F85" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="H85" s="5" t="str">
+      <c r="H85" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="82" Shortname="Tlxkpplng_" Duration="0" FunctionTypeCS2="Telexkupplung_hinten" FunctionTypeZ21="decouple" /&gt;</v>
       </c>
@@ -3676,10 +3690,10 @@
       <c r="E86" t="s">
         <v>92</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="H86" s="5" t="str">
+      <c r="H86" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="83" Shortname="Tlxkpplng_" Duration="0" FunctionTypeCS2="Telexkupplung_vorn" FunctionTypeZ21="decouple" /&gt;</v>
       </c>
@@ -3701,10 +3715,10 @@
       <c r="E87" t="s">
         <v>93</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F87" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="H87" s="5" t="str">
+      <c r="H87" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="84" Shortname="Pntgrph_hn" Duration="0" FunctionTypeCS2="Pantograph_hinten" FunctionTypeZ21="backward_take_power" /&gt;</v>
       </c>
@@ -3726,10 +3740,10 @@
       <c r="E88" t="s">
         <v>94</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="H88" s="5" t="str">
+      <c r="H88" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="85" Shortname="Pntgrph_vr" Duration="0" FunctionTypeCS2="Pantograph_vorne" FunctionTypeZ21="forward_take_power" /&gt;</v>
       </c>
@@ -3751,10 +3765,10 @@
       <c r="E89" t="s">
         <v>95</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F89" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="H89" s="5" t="str">
+      <c r="H89" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="86" Shortname="Frnlcht_hn" Duration="0" FunctionTypeCS2="Fernlicht_hinten" FunctionTypeZ21="main_beam" /&gt;</v>
       </c>
@@ -3776,10 +3790,10 @@
       <c r="E90" t="s">
         <v>96</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F90" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="H90" s="5" t="str">
+      <c r="H90" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="87" Shortname="Frnlcht_vr" Duration="0" FunctionTypeCS2="Fernlicht_vorn" FunctionTypeZ21="main_beam" /&gt;</v>
       </c>
@@ -3801,7 +3815,8 @@
       <c r="E91" t="s">
         <v>97</v>
       </c>
-      <c r="H91" s="5" t="str">
+      <c r="F91" s="7"/>
+      <c r="H91" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="88" Shortname="Shift" Duration="0" FunctionTypeCS2="Shift" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -3823,7 +3838,8 @@
       <c r="E92" t="s">
         <v>98</v>
       </c>
-      <c r="H92" s="5" t="str">
+      <c r="F92" s="7"/>
+      <c r="H92" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="89" Shortname="Vkmpmp" Duration="0" FunctionTypeCS2="Vakuumpumpe" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -3845,7 +3861,8 @@
       <c r="E93" t="s">
         <v>99</v>
       </c>
-      <c r="H93" s="5" t="str">
+      <c r="F93" s="7"/>
+      <c r="H93" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="90" Shortname="Trbwrksblc" Duration="0" FunctionTypeCS2="Triebwerksbeleuchtung" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -3867,10 +3884,10 @@
       <c r="E94" t="s">
         <v>100</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F94" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="H94" s="5" t="str">
+      <c r="H94" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="91" Shortname="Zylndr_sbl" Duration="0" FunctionTypeCS2="Zylinder_ausblasen_Dampf_ablassen" FunctionTypeZ21="dump_steam" /&gt;</v>
       </c>
@@ -3892,7 +3909,8 @@
       <c r="E95" t="s">
         <v>101</v>
       </c>
-      <c r="H95" s="5" t="str">
+      <c r="F95" s="7"/>
+      <c r="H95" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="92" Shortname="Drcklft_bl" Duration="0" FunctionTypeCS2="Druckluft_ablassen" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -3914,7 +3932,8 @@
       <c r="E96" t="s">
         <v>102</v>
       </c>
-      <c r="H96" s="5" t="str">
+      <c r="F96" s="7"/>
+      <c r="H96" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="93" Shortname="Kran" Duration="0" FunctionTypeCS2="Kran" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -3936,7 +3955,8 @@
       <c r="E97" t="s">
         <v>103</v>
       </c>
-      <c r="H97" s="5" t="str">
+      <c r="F97" s="7"/>
+      <c r="H97" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="94" Shortname="KrnBhn_f" Duration="0" FunctionTypeCS2="KranBuehne_auf" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -3958,7 +3978,8 @@
       <c r="E98" t="s">
         <v>104</v>
       </c>
-      <c r="H98" s="5" t="str">
+      <c r="F98" s="7"/>
+      <c r="H98" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="95" Shortname="KrnBhn_b" Duration="0" FunctionTypeCS2="KranBuehne_ab" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -3980,7 +4001,8 @@
       <c r="E99" t="s">
         <v>105</v>
       </c>
-      <c r="H99" s="5" t="str">
+      <c r="F99" s="7"/>
+      <c r="H99" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="96" Shortname="KrnBhn_lnk" Duration="0" FunctionTypeCS2="KranBuehne_links" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4002,7 +4024,8 @@
       <c r="E100" t="s">
         <v>106</v>
       </c>
-      <c r="H100" s="5" t="str">
+      <c r="F100" s="7"/>
+      <c r="H100" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="97" Shortname="KrnBhn_rch" Duration="0" FunctionTypeCS2="KranBuehne_rechts" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4024,7 +4047,8 @@
       <c r="E101" t="s">
         <v>107</v>
       </c>
-      <c r="H101" s="5" t="str">
+      <c r="F101" s="7"/>
+      <c r="H101" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="98" Shortname="KrnBhn_drh" Duration="0" FunctionTypeCS2="KranBuehne_drehen_rechts" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4046,7 +4070,8 @@
       <c r="E102" t="s">
         <v>108</v>
       </c>
-      <c r="H102" s="5" t="str">
+      <c r="F102" s="7"/>
+      <c r="H102" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="99" Shortname="Krn_Mgnt" Duration="0" FunctionTypeCS2="Kran_Magnet" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4068,7 +4093,8 @@
       <c r="E103" t="s">
         <v>109</v>
       </c>
-      <c r="H103" s="5" t="str">
+      <c r="F103" s="7"/>
+      <c r="H103" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="100" Shortname="Fhrtfrgb" Duration="0" FunctionTypeCS2="Fahrtfreigabe" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4090,7 +4116,8 @@
       <c r="E104" t="s">
         <v>110</v>
       </c>
-      <c r="H104" s="5" t="str">
+      <c r="F104" s="7"/>
+      <c r="H104" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="101" Shortname="Pntgrph_Af" Duration="0" FunctionTypeCS2="Pantograph_Auf_Abbuegelgeraeusch" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4112,7 +4139,8 @@
       <c r="E105" t="s">
         <v>111</v>
       </c>
-      <c r="H105" s="5" t="str">
+      <c r="F105" s="7"/>
+      <c r="H105" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="102" Shortname="Anfhr_Brms" Duration="0" FunctionTypeCS2="Anfahr_Bremsverzoegerung_ein" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4134,10 +4162,10 @@
       <c r="E106" t="s">
         <v>112</v>
       </c>
-      <c r="F106" t="s">
+      <c r="F106" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="H106" s="5" t="str">
+      <c r="H106" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="103" Shortname="Fnkgsprch" Duration="0" FunctionTypeCS2="Funkgespraech" FunctionTypeZ21="hump_funk" /&gt;</v>
       </c>
@@ -4159,10 +4187,10 @@
       <c r="E107" t="s">
         <v>113</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F107" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="H107" s="5" t="str">
+      <c r="H107" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="104" Shortname="Abfhrtsdrc" Duration="0" FunctionTypeCS2="Abfahrtsdurchsage" FunctionTypeZ21="sound1" /&gt;</v>
       </c>
@@ -4184,7 +4212,8 @@
       <c r="E108" t="s">
         <v>114</v>
       </c>
-      <c r="H108" s="5" t="str">
+      <c r="F108" s="7"/>
+      <c r="H108" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="105" Shortname="Assnblchtn" Duration="0" FunctionTypeCS2="Aussenbeleuchtung_Frontlicht" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4206,10 +4235,10 @@
       <c r="E109" t="s">
         <v>115</v>
       </c>
-      <c r="F109" t="s">
+      <c r="F109" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="H109" s="5" t="str">
+      <c r="H109" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="106" Shortname="Luftpumpe" Duration="0" FunctionTypeCS2="Luftpumpe" FunctionTypeZ21="air_pump" /&gt;</v>
       </c>
@@ -4231,7 +4260,8 @@
       <c r="E110" t="s">
         <v>116</v>
       </c>
-      <c r="H110" s="5" t="str">
+      <c r="F110" s="7"/>
+      <c r="H110" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="107" Shortname="Untrhltng_" Duration="0" FunctionTypeCS2="Unterhaltung_Allgemein" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4253,10 +4283,10 @@
       <c r="E111" t="s">
         <v>117</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F111" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="H111" s="5" t="str">
+      <c r="H111" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="108" Shortname="Sanden" Duration="0" FunctionTypeCS2="Sanden" FunctionTypeZ21="sanden" /&gt;</v>
       </c>
@@ -4278,10 +4308,10 @@
       <c r="E112" t="s">
         <v>118</v>
       </c>
-      <c r="F112" t="s">
+      <c r="F112" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="H112" s="5" t="str">
+      <c r="H112" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="109" Shortname="Mute_Fade" Duration="0" FunctionTypeCS2="Mute_Fade" FunctionTypeZ21="mute" /&gt;</v>
       </c>
@@ -4303,7 +4333,8 @@
       <c r="E113" t="s">
         <v>119</v>
       </c>
-      <c r="H113" s="5" t="str">
+      <c r="F113" s="7"/>
+      <c r="H113" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="110" Shortname="Trttstfnbl" Duration="0" FunctionTypeCS2="Trittstufenbeleuchtung" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4325,7 +4356,8 @@
       <c r="E114" t="s">
         <v>120</v>
       </c>
-      <c r="H114" s="5" t="str">
+      <c r="F114" s="7"/>
+      <c r="H114" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="111" Shortname="Spswssrpmp" Duration="0" FunctionTypeCS2="Speisewasserpumpe" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4347,7 +4379,8 @@
       <c r="E115" t="s">
         <v>121</v>
       </c>
-      <c r="H115" s="5" t="str">
+      <c r="F115" s="7"/>
+      <c r="H115" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="112" Shortname="Brmsnqtsch" Duration="0" FunctionTypeCS2="Bremsenquietschen_ein" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4369,7 +4402,8 @@
       <c r="E116" t="s">
         <v>122</v>
       </c>
-      <c r="H116" s="5" t="str">
+      <c r="F116" s="7"/>
+      <c r="H116" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="113" Shortname="Oelpumpe" Duration="0" FunctionTypeCS2="Oelpumpe" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4391,7 +4425,8 @@
       <c r="E117" t="s">
         <v>123</v>
       </c>
-      <c r="H117" s="5" t="str">
+      <c r="F117" s="7"/>
+      <c r="H117" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="114" Shortname="Schmrpmp" Duration="0" FunctionTypeCS2="Schmierpumpe" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4413,7 +4448,8 @@
       <c r="E118" t="s">
         <v>124</v>
       </c>
-      <c r="H118" s="5" t="str">
+      <c r="F118" s="7"/>
+      <c r="H118" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="115" Shortname="Dslpmp" Duration="0" FunctionTypeCS2="Dieselpumpe" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4435,10 +4471,10 @@
       <c r="E119" t="s">
         <v>125</v>
       </c>
-      <c r="F119" t="s">
+      <c r="F119" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="H119" s="5" t="str">
+      <c r="H119" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="116" Shortname="Kompressor" Duration="0" FunctionTypeCS2="Kompressor" FunctionTypeZ21="compressor" /&gt;</v>
       </c>
@@ -4460,7 +4496,8 @@
       <c r="E120" t="s">
         <v>126</v>
       </c>
-      <c r="H120" s="5" t="str">
+      <c r="F120" s="7"/>
+      <c r="H120" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="117" Shortname="Knslnblcht" Duration="0" FunctionTypeCS2="Konsolenbeleuchtung" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4482,10 +4519,10 @@
       <c r="E121" t="s">
         <v>127</v>
       </c>
-      <c r="F121" t="s">
+      <c r="F121" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="H121" s="5" t="str">
+      <c r="H121" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="118" Shortname="Rngrblchtn" Duration="0" FunctionTypeCS2="Rangierbeleuchtung" FunctionTypeZ21="sidelights" /&gt;</v>
       </c>
@@ -4507,7 +4544,8 @@
       <c r="E122" t="s">
         <v>128</v>
       </c>
-      <c r="H122" s="5" t="str">
+      <c r="F122" s="7"/>
+      <c r="H122" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="119" Shortname="Prtyblchtn" Duration="0" FunctionTypeCS2="Partybeleuchtung" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4529,7 +4567,8 @@
       <c r="E123" t="s">
         <v>129</v>
       </c>
-      <c r="H123" s="5" t="str">
+      <c r="F123" s="7"/>
+      <c r="H123" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="120" Shortname="Wrtnd_Pssg" Duration="0" FunctionTypeCS2="Wartende_Passagiere" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4551,10 +4590,10 @@
       <c r="E124" t="s">
         <v>130</v>
       </c>
-      <c r="F124" t="s">
+      <c r="F124" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="H124" s="5" t="str">
+      <c r="H124" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="121" Shortname="Anknft_Zln" Duration="0" FunctionTypeCS2="Ankunft_Zielansage" FunctionTypeZ21="sound1" /&gt;</v>
       </c>
@@ -4576,10 +4615,10 @@
       <c r="E125" t="s">
         <v>131</v>
       </c>
-      <c r="F125" t="s">
+      <c r="F125" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="H125" s="5" t="str">
+      <c r="H125" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="122" Shortname="Zgnsg_Schf" Duration="0" FunctionTypeCS2="Zugansage_Schaffener" FunctionTypeZ21="sound3" /&gt;</v>
       </c>
@@ -4601,7 +4640,8 @@
       <c r="E126" t="s">
         <v>132</v>
       </c>
-      <c r="H126" s="5" t="str">
+      <c r="F126" s="7"/>
+      <c r="H126" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="123" Shortname="Schrhtsvnt" Duration="0" FunctionTypeCS2="Sicherheitsventil" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4623,7 +4663,8 @@
       <c r="E127" t="s">
         <v>133</v>
       </c>
-      <c r="H127" s="5" t="str">
+      <c r="F127" s="7"/>
+      <c r="H127" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="124" Shortname="Ksslhzng" Duration="0" FunctionTypeCS2="Kesselheizung" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4645,7 +4686,8 @@
       <c r="E128" t="s">
         <v>134</v>
       </c>
-      <c r="H128" s="5" t="str">
+      <c r="F128" s="7"/>
+      <c r="H128" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="125" Shortname="Hlfsggrgt_" Duration="0" FunctionTypeCS2="Hilfsaggregat_Hilfsdiesel" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4667,10 +4709,10 @@
       <c r="E129" t="s">
         <v>135</v>
       </c>
-      <c r="F129" t="s">
+      <c r="F129" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="H129" s="5" t="str">
+      <c r="H129" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="126" Shortname="Mschnnrmbl" Duration="0" FunctionTypeCS2="Maschinenraumbeleuchtung" FunctionTypeZ21="cycle_light" /&gt;</v>
       </c>
@@ -4692,10 +4734,10 @@
       <c r="E130" t="s">
         <v>136</v>
       </c>
-      <c r="F130" t="s">
+      <c r="F130" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="H130" s="5" t="str">
+      <c r="H130" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="127" Shortname="Partymusik" Duration="0" FunctionTypeCS2="Partymusik" FunctionTypeZ21="clef" /&gt;</v>
       </c>
@@ -4717,10 +4759,10 @@
       <c r="E131" t="s">
         <v>137</v>
       </c>
-      <c r="F131" t="s">
+      <c r="F131" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="H131" s="5" t="str">
+      <c r="H131" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="128" Shortname="Krvngrsch" Duration="0" FunctionTypeCS2="Kurvengeraeusch" FunctionTypeZ21="curve_sound" /&gt;</v>
       </c>
@@ -4742,7 +4784,8 @@
       <c r="E132" t="s">
         <v>138</v>
       </c>
-      <c r="H132" s="5" t="str">
+      <c r="F132" s="7"/>
+      <c r="H132" s="8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;mapping Id="129" Shortname="Blinker" Duration="0" FunctionTypeCS2="Blinker" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4764,10 +4807,10 @@
       <c r="E133" t="s">
         <v>139</v>
       </c>
-      <c r="F133" t="s">
+      <c r="F133" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="H133" s="5" t="str">
+      <c r="H133" s="8" t="str">
         <f t="shared" ref="H133:H196" si="5">"&lt;mapping Id="""&amp;A133&amp;""" Shortname="""&amp;B133&amp;""" Duration="""&amp;C133&amp;""" FunctionTypeCS2="""&amp;E133&amp;""" FunctionTypeZ21="""&amp;F133&amp;""" /&gt;"</f>
         <v>&lt;mapping Id="130" Shortname="Ablssvntl" Duration="0" FunctionTypeCS2="Ablassventil" FunctionTypeZ21="drain_valve" /&gt;</v>
       </c>
@@ -4789,7 +4832,8 @@
       <c r="E134" t="s">
         <v>140</v>
       </c>
-      <c r="H134" s="5" t="str">
+      <c r="F134" s="7"/>
+      <c r="H134" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="131" Shortname="Wrnmldngn" Duration="0" FunctionTypeCS2="Warnmeldungen" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4811,7 +4855,8 @@
       <c r="E135" t="s">
         <v>141</v>
       </c>
-      <c r="H135" s="5" t="str">
+      <c r="F135" s="7"/>
+      <c r="H135" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="132" Shortname="Fhrrstndsg" Duration="0" FunctionTypeCS2="Fuehrerstandsgespraech" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4833,7 +4878,8 @@
       <c r="E136" t="s">
         <v>142</v>
       </c>
-      <c r="H136" s="5" t="str">
+      <c r="F136" s="7"/>
+      <c r="H136" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="133" Shortname="Infrmtnsdr" Duration="0" FunctionTypeCS2="Informationsdurchsage" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4855,7 +4901,8 @@
       <c r="E137" t="s">
         <v>143</v>
       </c>
-      <c r="H137" s="5" t="str">
+      <c r="F137" s="7"/>
+      <c r="H137" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="134" Shortname="Snstg_Pmp" Duration="0" FunctionTypeCS2="Sonstige_Pumpe" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4877,7 +4924,8 @@
       <c r="E138" t="s">
         <v>144</v>
       </c>
-      <c r="H138" s="5" t="str">
+      <c r="F138" s="7"/>
+      <c r="H138" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="135" Shortname="Kmbntn_sch" Duration="0" FunctionTypeCS2="Kombination_schaufeln_Feuerbuechse" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4899,7 +4947,8 @@
       <c r="E139" t="s">
         <v>145</v>
       </c>
-      <c r="H139" s="5" t="str">
+      <c r="F139" s="7"/>
+      <c r="H139" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="136" Shortname="Bwglchr_Sc" Duration="0" FunctionTypeCS2="Beweglicher_Schaffner" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4921,7 +4970,8 @@
       <c r="E140" t="s">
         <v>146</v>
       </c>
-      <c r="H140" s="5" t="str">
+      <c r="F140" s="7"/>
+      <c r="H140" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="137" Shortname="Fnstr_f_z" Duration="0" FunctionTypeCS2="Fenster_auf_zu" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4943,7 +4993,8 @@
       <c r="E141" t="s">
         <v>147</v>
       </c>
-      <c r="H141" s="5" t="str">
+      <c r="F141" s="7"/>
+      <c r="H141" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="138" Shortname="Grsch_Fnst" Duration="0" FunctionTypeCS2="Geraeusch_Fenster_auf_zu" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4965,7 +5016,8 @@
       <c r="E142" t="s">
         <v>148</v>
       </c>
-      <c r="H142" s="5" t="str">
+      <c r="F142" s="7"/>
+      <c r="H142" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="139" Shortname="Drchsg_Trn" Duration="0" FunctionTypeCS2="Durchsage_Tueren_schlissen_rechts" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -4987,7 +5039,8 @@
       <c r="E143" t="s">
         <v>149</v>
       </c>
-      <c r="H143" s="5" t="str">
+      <c r="F143" s="7"/>
+      <c r="H143" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="140" Shortname="Ambnt_Stdt" Duration="0" FunctionTypeCS2="Ambiente_Stadt" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5009,7 +5062,8 @@
       <c r="E144" t="s">
         <v>150</v>
       </c>
-      <c r="H144" s="5" t="str">
+      <c r="F144" s="7"/>
+      <c r="H144" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="141" Shortname="Ambnt_Tnnl" Duration="0" FunctionTypeCS2="Ambiente_Tunnel" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5031,7 +5085,8 @@
       <c r="E145" t="s">
         <v>151</v>
       </c>
-      <c r="H145" s="5" t="str">
+      <c r="F145" s="7"/>
+      <c r="H145" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="142" Shortname="Ambnt_Sthl" Duration="0" FunctionTypeCS2="Ambiente_Stahlbruecke" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5053,7 +5108,8 @@
       <c r="E146" t="s">
         <v>152</v>
       </c>
-      <c r="H146" s="5" t="str">
+      <c r="F146" s="7"/>
+      <c r="H146" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="143" Shortname="Ambnt_Btnb" Duration="0" FunctionTypeCS2="Ambiente_Betonbruecke" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5075,7 +5131,8 @@
       <c r="E147" t="s">
         <v>153</v>
       </c>
-      <c r="H147" s="5" t="str">
+      <c r="F147" s="7"/>
+      <c r="H147" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="144" Shortname="Grsch_Klpp" Duration="0" FunctionTypeCS2="Geraeusch_Klapptuere" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5097,7 +5154,8 @@
       <c r="E148" t="s">
         <v>154</v>
       </c>
-      <c r="H148" s="5" t="str">
+      <c r="F148" s="7"/>
+      <c r="H148" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="145" Shortname="Grsch_Tr" Duration="0" FunctionTypeCS2="Geraeusch_Tuere" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5119,7 +5177,8 @@
       <c r="E149" t="s">
         <v>155</v>
       </c>
-      <c r="H149" s="5" t="str">
+      <c r="F149" s="7"/>
+      <c r="H149" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="146" Shortname="Grsch_Fllt" Duration="0" FunctionTypeCS2="Geraeusch_Falltuere" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5141,7 +5200,8 @@
       <c r="E150" t="s">
         <v>156</v>
       </c>
-      <c r="H150" s="5" t="str">
+      <c r="F150" s="7"/>
+      <c r="H150" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="147" Shortname="Glck_krz" Duration="0" FunctionTypeCS2="Glocke_kurz" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5163,7 +5223,8 @@
       <c r="E151" t="s">
         <v>157</v>
       </c>
-      <c r="H151" s="5" t="str">
+      <c r="F151" s="7"/>
+      <c r="H151" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="148" Shortname="Grsch_Rllt" Duration="0" FunctionTypeCS2="Geraeusch_Rolltor" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5185,7 +5246,8 @@
       <c r="E152" t="s">
         <v>158</v>
       </c>
-      <c r="H152" s="5" t="str">
+      <c r="F152" s="7"/>
+      <c r="H152" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="149" Shortname="Grsch_Schb" Duration="0" FunctionTypeCS2="Geraeusch_Schiebetuer" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5207,7 +5269,8 @@
       <c r="E153" t="s">
         <v>159</v>
       </c>
-      <c r="H153" s="5" t="str">
+      <c r="F153" s="7"/>
+      <c r="H153" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="150" Shortname="Dampfstoss" Duration="0" FunctionTypeCS2="Dampfstoss" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5229,7 +5292,8 @@
       <c r="E154" t="s">
         <v>160</v>
       </c>
-      <c r="H154" s="5" t="str">
+      <c r="F154" s="7"/>
+      <c r="H154" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="151" Shortname="Dslhzng" Duration="0" FunctionTypeCS2="Dieselheizung" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5251,7 +5315,8 @@
       <c r="E155" t="s">
         <v>161</v>
       </c>
-      <c r="H155" s="5" t="str">
+      <c r="F155" s="7"/>
+      <c r="H155" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="152" Shortname="Zugheizung" Duration="0" FunctionTypeCS2="Zugheizung" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5273,7 +5338,8 @@
       <c r="E156" t="s">
         <v>162</v>
       </c>
-      <c r="H156" s="5" t="str">
+      <c r="F156" s="7"/>
+      <c r="H156" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="153" Shortname="Segeln" Duration="0" FunctionTypeCS2="Segeln" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5295,10 +5361,10 @@
       <c r="E157" t="s">
         <v>163</v>
       </c>
-      <c r="F157" t="s">
+      <c r="F157" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="H157" s="5" t="str">
+      <c r="H157" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="154" Shortname="Zg_Infnsg" Duration="0" FunctionTypeCS2="Zug_Infoansage" FunctionTypeZ21="sound1" /&gt;</v>
       </c>
@@ -5320,7 +5386,8 @@
       <c r="E158" t="s">
         <v>164</v>
       </c>
-      <c r="H158" s="5" t="str">
+      <c r="F158" s="7"/>
+      <c r="H158" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="155" Shortname="Sndrnsg" Duration="0" FunctionTypeCS2="Sonderansage" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5342,7 +5409,8 @@
       <c r="E159" t="s">
         <v>165</v>
       </c>
-      <c r="H159" s="5" t="str">
+      <c r="F159" s="7"/>
+      <c r="H159" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="156" Shortname="Wrtnd_Pssg" Duration="0" FunctionTypeCS2="Wartende_Passagiere_am_Bahnhof" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5364,7 +5432,8 @@
       <c r="E160" t="s">
         <v>166</v>
       </c>
-      <c r="H160" s="5" t="str">
+      <c r="F160" s="7"/>
+      <c r="H160" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="157" Shortname="Bocksprung" Duration="0" FunctionTypeCS2="Bocksprung" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5386,7 +5455,8 @@
       <c r="E161" t="s">
         <v>167</v>
       </c>
-      <c r="H161" s="5" t="str">
+      <c r="F161" s="7"/>
+      <c r="H161" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="158" Shortname="Drchsg_Trn" Duration="0" FunctionTypeCS2="Durchsage_Tueren_schlissen_links" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5408,7 +5478,8 @@
       <c r="E162" t="s">
         <v>168</v>
       </c>
-      <c r="H162" s="5" t="str">
+      <c r="F162" s="7"/>
+      <c r="H162" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="159" Shortname="Zuggattung" Duration="0" FunctionTypeCS2="Zuggattung" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5430,7 +5501,8 @@
       <c r="E163" t="s">
         <v>169</v>
       </c>
-      <c r="H163" s="5" t="str">
+      <c r="F163" s="7"/>
+      <c r="H163" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="160" Shortname="Zgdrchsg" Duration="0" FunctionTypeCS2="Zugdurchsage" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5452,10 +5524,10 @@
       <c r="E164" t="s">
         <v>170</v>
       </c>
-      <c r="F164" t="s">
+      <c r="F164" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="H164" s="5" t="str">
+      <c r="H164" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="161" Shortname="Wrnblnklch" Duration="0" FunctionTypeCS2="Warnblinklicht" FunctionTypeZ21="all_round_light" /&gt;</v>
       </c>
@@ -5477,7 +5549,8 @@
       <c r="E165" t="s">
         <v>171</v>
       </c>
-      <c r="H165" s="5" t="str">
+      <c r="F165" s="7"/>
+      <c r="H165" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="162" Shortname="Play" Duration="0" FunctionTypeCS2="Play" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5499,7 +5572,8 @@
       <c r="E166" t="s">
         <v>172</v>
       </c>
-      <c r="H166" s="5" t="str">
+      <c r="F166" s="7"/>
+      <c r="H166" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="163" Shortname="Pause" Duration="0" FunctionTypeCS2="Pause" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5521,7 +5595,8 @@
       <c r="E167" t="s">
         <v>173</v>
       </c>
-      <c r="H167" s="5" t="str">
+      <c r="F167" s="7"/>
+      <c r="H167" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="164" Shortname="Vor" Duration="0" FunctionTypeCS2="Vor" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5543,7 +5618,8 @@
       <c r="E168" t="s">
         <v>174</v>
       </c>
-      <c r="H168" s="5" t="str">
+      <c r="F168" s="7"/>
+      <c r="H168" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="165" Shortname="Zurueck" Duration="0" FunctionTypeCS2="Zurueck" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5565,10 +5641,10 @@
       <c r="E169" t="s">
         <v>175</v>
       </c>
-      <c r="F169" t="s">
+      <c r="F169" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="H169" s="5" t="str">
+      <c r="H169" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="166" Shortname="Laut" Duration="0" FunctionTypeCS2="Laut" FunctionTypeZ21="louder" /&gt;</v>
       </c>
@@ -5590,10 +5666,10 @@
       <c r="E170" t="s">
         <v>176</v>
       </c>
-      <c r="F170" t="s">
+      <c r="F170" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="H170" s="5" t="str">
+      <c r="H170" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="167" Shortname="Leise" Duration="0" FunctionTypeCS2="Leise" FunctionTypeZ21="quieter" /&gt;</v>
       </c>
@@ -5615,7 +5691,8 @@
       <c r="E171" t="s">
         <v>177</v>
       </c>
-      <c r="H171" s="5" t="str">
+      <c r="F171" s="7"/>
+      <c r="H171" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="168" Shortname="Lcht_Abtl" Duration="0" FunctionTypeCS2="Licht_Abteile" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5637,7 +5714,8 @@
       <c r="E172" t="s">
         <v>178</v>
       </c>
-      <c r="H172" s="5" t="str">
+      <c r="F172" s="7"/>
+      <c r="H172" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="169" Shortname="Licht_Gang" Duration="0" FunctionTypeCS2="Licht_Gang" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5659,7 +5737,8 @@
       <c r="E173" t="s">
         <v>179</v>
       </c>
-      <c r="H173" s="5" t="str">
+      <c r="F173" s="7"/>
+      <c r="H173" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="170" Shortname="Lcht_Kch" Duration="0" FunctionTypeCS2="Licht_Kueche" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5681,7 +5760,8 @@
       <c r="E174" t="s">
         <v>180</v>
       </c>
-      <c r="H174" s="5" t="str">
+      <c r="F174" s="7"/>
+      <c r="H174" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="171" Shortname="Lcht_Gpck" Duration="0" FunctionTypeCS2="Licht_Gepaeck" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5703,7 +5783,8 @@
       <c r="E175" t="s">
         <v>181</v>
       </c>
-      <c r="H175" s="5" t="str">
+      <c r="F175" s="7"/>
+      <c r="H175" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="172" Shortname="Licht_Bar" Duration="0" FunctionTypeCS2="Licht_Bar" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5725,7 +5806,8 @@
       <c r="E176" t="s">
         <v>182</v>
       </c>
-      <c r="H176" s="5" t="str">
+      <c r="F176" s="7"/>
+      <c r="H176" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="173" Shortname="Tanken" Duration="0" FunctionTypeCS2="Tanken" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5747,7 +5829,8 @@
       <c r="E177" t="s">
         <v>183</v>
       </c>
-      <c r="H177" s="5" t="str">
+      <c r="F177" s="7"/>
+      <c r="H177" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="174" Shortname="Wasser" Duration="0" FunctionTypeCS2="Wasser" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5769,7 +5852,8 @@
       <c r="E178" t="s">
         <v>184</v>
       </c>
-      <c r="H178" s="5" t="str">
+      <c r="F178" s="7"/>
+      <c r="H178" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="175" Shortname="Diesel" Duration="0" FunctionTypeCS2="Diesel" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5791,7 +5875,8 @@
       <c r="E179" t="s">
         <v>185</v>
       </c>
-      <c r="H179" s="5" t="str">
+      <c r="F179" s="7"/>
+      <c r="H179" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="176" Shortname="Kohle" Duration="0" FunctionTypeCS2="Kohle" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5813,7 +5898,8 @@
       <c r="E180" t="s">
         <v>186</v>
       </c>
-      <c r="H180" s="5" t="str">
+      <c r="F180" s="7"/>
+      <c r="H180" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="177" Shortname="Khlstb_2" Duration="0" FunctionTypeCS2="Kohlestaub_2" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5835,7 +5921,8 @@
       <c r="E181" t="s">
         <v>187</v>
       </c>
-      <c r="H181" s="5" t="str">
+      <c r="F181" s="7"/>
+      <c r="H181" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="178" Shortname="Oel" Duration="0" FunctionTypeCS2="Oel" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5857,7 +5944,8 @@
       <c r="E182" t="s">
         <v>188</v>
       </c>
-      <c r="H182" s="5" t="str">
+      <c r="F182" s="7"/>
+      <c r="H182" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="179" Shortname="Sand" Duration="0" FunctionTypeCS2="Sand" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5879,10 +5967,10 @@
       <c r="E183" t="s">
         <v>189</v>
       </c>
-      <c r="F183" t="s">
+      <c r="F183" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="H183" s="5" t="str">
+      <c r="H183" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="180" Shortname="Schwzr_Lch" Duration="0" FunctionTypeCS2="Schweizer_Lichtwechsel" FunctionTypeZ21="coach_side_light_off" /&gt;</v>
       </c>
@@ -5904,7 +5992,8 @@
       <c r="E184" t="s">
         <v>190</v>
       </c>
-      <c r="H184" s="5" t="str">
+      <c r="F184" s="7"/>
+      <c r="H184" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="181" Shortname="Ansg_Pfff_" Duration="0" FunctionTypeCS2="Ansage_Pfiff_mit_Tuerschliessen" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5926,7 +6015,8 @@
       <c r="E185" t="s">
         <v>191</v>
       </c>
-      <c r="H185" s="5" t="str">
+      <c r="F185" s="7"/>
+      <c r="H185" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="182" Shortname="Zufall_Aus" Duration="0" FunctionTypeCS2="Zufall_Aus" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5948,7 +6038,8 @@
       <c r="E186" t="s">
         <v>192</v>
       </c>
-      <c r="H186" s="5" t="str">
+      <c r="F186" s="7"/>
+      <c r="H186" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="183" Shortname="Sifataster" Duration="0" FunctionTypeCS2="Sifataster" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5970,7 +6061,8 @@
       <c r="E187" t="s">
         <v>193</v>
       </c>
-      <c r="H187" s="5" t="str">
+      <c r="F187" s="7"/>
+      <c r="H187" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="184" Shortname="Not_Aus" Duration="0" FunctionTypeCS2="Not_Aus" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -5992,7 +6084,8 @@
       <c r="E188" t="s">
         <v>194</v>
       </c>
-      <c r="H188" s="5" t="str">
+      <c r="F188" s="7"/>
+      <c r="H188" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="185" Shortname="Schalter" Duration="0" FunctionTypeCS2="Schalter" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6014,7 +6107,8 @@
       <c r="E189" t="s">
         <v>195</v>
       </c>
-      <c r="H189" s="5" t="str">
+      <c r="F189" s="7"/>
+      <c r="H189" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="186" Shortname="Kppschltr" Duration="0" FunctionTypeCS2="Kippschlater" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6036,7 +6130,8 @@
       <c r="E190" t="s">
         <v>196</v>
       </c>
-      <c r="H190" s="5" t="str">
+      <c r="F190" s="7"/>
+      <c r="H190" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="187" Shortname="Drhschltr" Duration="0" FunctionTypeCS2="Drehschalter" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6058,7 +6153,8 @@
       <c r="E191" t="s">
         <v>197</v>
       </c>
-      <c r="H191" s="5" t="str">
+      <c r="F191" s="7"/>
+      <c r="H191" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="188" Shortname="Not_Halt" Duration="0" FunctionTypeCS2="Not_Halt" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6080,7 +6176,8 @@
       <c r="E192" t="s">
         <v>198</v>
       </c>
-      <c r="H192" s="5" t="str">
+      <c r="F192" s="7"/>
+      <c r="H192" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="189" Shortname="Snd_Zhnrd" Duration="0" FunctionTypeCS2="Sound_Zahnrad" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6102,7 +6199,8 @@
       <c r="E193" t="s">
         <v>199</v>
       </c>
-      <c r="H193" s="5" t="str">
+      <c r="F193" s="7"/>
+      <c r="H193" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="190" Shortname="Klckrn_Tch" Duration="0" FunctionTypeCS2="Klackern_Tacho" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6124,7 +6222,8 @@
       <c r="E194" t="s">
         <v>200</v>
       </c>
-      <c r="H194" s="5" t="str">
+      <c r="F194" s="7"/>
+      <c r="H194" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="191" Shortname="Snd_Wschr" Duration="0" FunctionTypeCS2="Sound_Wischer" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6146,7 +6245,8 @@
       <c r="E195" t="s">
         <v>201</v>
       </c>
-      <c r="H195" s="5" t="str">
+      <c r="F195" s="7"/>
+      <c r="H195" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="192" Shortname="Zhnrd_Antr" Duration="0" FunctionTypeCS2="Zahnrad_Antrieb" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6168,7 +6268,8 @@
       <c r="E196" t="s">
         <v>202</v>
       </c>
-      <c r="H196" s="5" t="str">
+      <c r="F196" s="7"/>
+      <c r="H196" s="8" t="str">
         <f t="shared" si="5"/>
         <v>&lt;mapping Id="193" Shortname="Wischer" Duration="0" FunctionTypeCS2="Wischer" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6190,7 +6291,8 @@
       <c r="E197" t="s">
         <v>203</v>
       </c>
-      <c r="H197" s="5" t="str">
+      <c r="F197" s="7"/>
+      <c r="H197" s="8" t="str">
         <f t="shared" ref="H197:H234" si="7">"&lt;mapping Id="""&amp;A197&amp;""" Shortname="""&amp;B197&amp;""" Duration="""&amp;C197&amp;""" FunctionTypeCS2="""&amp;E197&amp;""" FunctionTypeZ21="""&amp;F197&amp;""" /&gt;"</f>
         <v>&lt;mapping Id="194" Shortname="Abschlmmn_" Duration="0" FunctionTypeCS2="Abschlammen_Schlaemmen" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6212,7 +6314,8 @@
       <c r="E198" t="s">
         <v>204</v>
       </c>
-      <c r="H198" s="5" t="str">
+      <c r="F198" s="7"/>
+      <c r="H198" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="195" Shortname="Glck_lng" Duration="0" FunctionTypeCS2="Glocke_lang" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6234,10 +6337,10 @@
       <c r="E199" t="s">
         <v>205</v>
       </c>
-      <c r="F199" t="s">
+      <c r="F199" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="H199" s="5" t="str">
+      <c r="H199" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="196" Shortname="Horn_kurz" Duration="0" FunctionTypeCS2="Horn_kurz" FunctionTypeZ21="horn_high" /&gt;</v>
       </c>
@@ -6259,10 +6362,10 @@
       <c r="E200" t="s">
         <v>206</v>
       </c>
-      <c r="F200" t="s">
+      <c r="F200" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="H200" s="5" t="str">
+      <c r="H200" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="197" Shortname="Horn_lang" Duration="0" FunctionTypeCS2="Horn_lang" FunctionTypeZ21="horn_low" /&gt;</v>
       </c>
@@ -6284,10 +6387,10 @@
       <c r="E201" t="s">
         <v>207</v>
       </c>
-      <c r="F201" t="s">
+      <c r="F201" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="H201" s="5" t="str">
+      <c r="H201" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="198" Shortname="Pff_krz" Duration="0" FunctionTypeCS2="Pfeife_kurz" FunctionTypeZ21="whistle_short" /&gt;</v>
       </c>
@@ -6309,10 +6412,10 @@
       <c r="E202" t="s">
         <v>208</v>
       </c>
-      <c r="F202" t="s">
+      <c r="F202" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H202" s="5" t="str">
+      <c r="H202" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="199" Shortname="Pff_lng" Duration="0" FunctionTypeCS2="Pfeife_lang" FunctionTypeZ21="whistle_long" /&gt;</v>
       </c>
@@ -6334,7 +6437,8 @@
       <c r="E203" t="s">
         <v>209</v>
       </c>
-      <c r="H203" s="5" t="str">
+      <c r="F203" s="7"/>
+      <c r="H203" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="200" Shortname="Krn_En_Ums" Duration="0" FunctionTypeCS2="Kran_Ein_Umschalten_Fahrbetrieb_Funktionsbetrieb" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6356,7 +6460,8 @@
       <c r="E204" t="s">
         <v>210</v>
       </c>
-      <c r="H204" s="5" t="str">
+      <c r="F204" s="7"/>
+      <c r="H204" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="201" Shortname="Krn_As_Grn" Duration="0" FunctionTypeCS2="Kran_Aus_Grundstellung_anfahren" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6378,7 +6483,8 @@
       <c r="E205" t="s">
         <v>211</v>
       </c>
-      <c r="H205" s="5" t="str">
+      <c r="F205" s="7"/>
+      <c r="H205" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="202" Shortname="Kran_Haken" Duration="0" FunctionTypeCS2="Kran_Haken" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6400,7 +6506,8 @@
       <c r="E206" t="s">
         <v>212</v>
       </c>
-      <c r="H206" s="5" t="str">
+      <c r="F206" s="7"/>
+      <c r="H206" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="203" Shortname="Hammer" Duration="0" FunctionTypeCS2="Hammer" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6422,7 +6529,8 @@
       <c r="E207" t="s">
         <v>213</v>
       </c>
-      <c r="H207" s="5" t="str">
+      <c r="F207" s="7"/>
+      <c r="H207" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="204" Shortname="Saege" Duration="0" FunctionTypeCS2="Saege" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6444,7 +6552,8 @@
       <c r="E208" t="s">
         <v>214</v>
       </c>
-      <c r="H208" s="5" t="str">
+      <c r="F208" s="7"/>
+      <c r="H208" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="205" Shortname="Bhrmschn_B" Duration="0" FunctionTypeCS2="Bohrmaschine_Bohrer" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6466,7 +6575,8 @@
       <c r="E209" t="s">
         <v>215</v>
       </c>
-      <c r="H209" s="5" t="str">
+      <c r="F209" s="7"/>
+      <c r="H209" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="206" Shortname="Schwssgrt_" Duration="0" FunctionTypeCS2="Schweissgeraet_Schweissen" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6488,7 +6598,8 @@
       <c r="E210" t="s">
         <v>216</v>
       </c>
-      <c r="H210" s="5" t="str">
+      <c r="F210" s="7"/>
+      <c r="H210" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="207" Shortname="Schlfblck_" Duration="0" FunctionTypeCS2="Schleifblock_Schleifen" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6510,7 +6621,8 @@
       <c r="E211" t="s">
         <v>217</v>
       </c>
-      <c r="H211" s="5" t="str">
+      <c r="F211" s="7"/>
+      <c r="H211" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="208" Shortname="Drhtbrst_B" Duration="0" FunctionTypeCS2="Drahtbuerste_Buersten" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6532,7 +6644,8 @@
       <c r="E212" t="s">
         <v>218</v>
       </c>
-      <c r="H212" s="5" t="str">
+      <c r="F212" s="7"/>
+      <c r="H212" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="209" Shortname="Kettenzug" Duration="0" FunctionTypeCS2="Kettenzug" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6554,7 +6667,8 @@
       <c r="E213" t="s">
         <v>219</v>
       </c>
-      <c r="H213" s="5" t="str">
+      <c r="F213" s="7"/>
+      <c r="H213" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="210" Shortname="Trnnschlfr" Duration="0" FunctionTypeCS2="Trennschleifer_Flex" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6576,7 +6690,8 @@
       <c r="E214" t="s">
         <v>220</v>
       </c>
-      <c r="H214" s="5" t="str">
+      <c r="F214" s="7"/>
+      <c r="H214" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="211" Shortname="Schaufel" Duration="0" FunctionTypeCS2="Schaufel" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6598,7 +6713,8 @@
       <c r="E215" t="s">
         <v>221</v>
       </c>
-      <c r="H215" s="5" t="str">
+      <c r="F215" s="7"/>
+      <c r="H215" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="212" Shortname="Ldn_Enldn_" Duration="0" FunctionTypeCS2="Laden_Einladen_Ausladen" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6620,7 +6736,8 @@
       <c r="E216" t="s">
         <v>222</v>
       </c>
-      <c r="H216" s="5" t="str">
+      <c r="F216" s="7"/>
+      <c r="H216" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="213" Shortname="Prsslfthmm" Duration="0" FunctionTypeCS2="Presslufthammer_Hämmern" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6642,7 +6759,8 @@
       <c r="E217" t="s">
         <v>223</v>
       </c>
-      <c r="H217" s="5" t="str">
+      <c r="F217" s="7"/>
+      <c r="H217" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="214" Shortname="Stop" Duration="0" FunctionTypeCS2="Stop" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6664,7 +6782,8 @@
       <c r="E218" t="s">
         <v>224</v>
       </c>
-      <c r="H218" s="5" t="str">
+      <c r="F218" s="7"/>
+      <c r="H218" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="215" Shortname="Naechstes" Duration="0" FunctionTypeCS2="Naechstes" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6686,7 +6805,8 @@
       <c r="E219" t="s">
         <v>225</v>
       </c>
-      <c r="H219" s="5" t="str">
+      <c r="F219" s="7"/>
+      <c r="H219" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="216" Shortname="Letztes" Duration="0" FunctionTypeCS2="Letztes" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6708,7 +6828,8 @@
       <c r="E220" t="s">
         <v>226</v>
       </c>
-      <c r="H220" s="5" t="str">
+      <c r="F220" s="7"/>
+      <c r="H220" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="217" Shortname="Bhnbrgng" Duration="0" FunctionTypeCS2="Bahnuebergang" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6730,7 +6851,8 @@
       <c r="E221" t="s">
         <v>227</v>
       </c>
-      <c r="H221" s="5" t="str">
+      <c r="F221" s="7"/>
+      <c r="H221" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="218" Shortname="Glck_Bhnbr" Duration="0" FunctionTypeCS2="Glocke_Bahnuebergang" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6752,10 +6874,10 @@
       <c r="E222" t="s">
         <v>228</v>
       </c>
-      <c r="F222" t="s">
+      <c r="F222" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="H222" s="5" t="str">
+      <c r="H222" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="219" Shortname="Strklftn" Duration="0" FunctionTypeCS2="Starklueften" FunctionTypeZ21="fan_strong" /&gt;</v>
       </c>
@@ -6777,10 +6899,10 @@
       <c r="E223" t="s">
         <v>229</v>
       </c>
-      <c r="F223" t="s">
+      <c r="F223" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="H223" s="5" t="str">
+      <c r="H223" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="220" Shortname="Schwchlftn" Duration="0" FunctionTypeCS2="Schwachlueften" FunctionTypeZ21="fan" /&gt;</v>
       </c>
@@ -6802,10 +6924,10 @@
       <c r="E224" t="s">
         <v>230</v>
       </c>
-      <c r="F224" t="s">
+      <c r="F224" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="H224" s="5" t="str">
+      <c r="H224" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="221" Shortname="Tlx_Wlzr" Duration="0" FunctionTypeCS2="Telex_Walzer" FunctionTypeZ21="decouple" /&gt;</v>
       </c>
@@ -6827,10 +6949,10 @@
       <c r="E225" t="s">
         <v>231</v>
       </c>
-      <c r="F225" t="s">
+      <c r="F225" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="H225" s="5" t="str">
+      <c r="H225" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="222" Shortname="Lcht_Gnrtr" Duration="0" FunctionTypeCS2="Licht_Generator_Sound" FunctionTypeZ21="alternator" /&gt;</v>
       </c>
@@ -6852,7 +6974,8 @@
       <c r="E226" t="s">
         <v>232</v>
       </c>
-      <c r="H226" s="5" t="str">
+      <c r="F226" s="7"/>
+      <c r="H226" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="223" Shortname="Rchkmmr" Duration="0" FunctionTypeCS2="Rauchkammer" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6874,7 +6997,8 @@
       <c r="E227" t="s">
         <v>233</v>
       </c>
-      <c r="H227" s="5" t="str">
+      <c r="F227" s="7"/>
+      <c r="H227" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="224" Shortname="Kohlestaub" Duration="0" FunctionTypeCS2="Kohlestaub" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6896,7 +7020,8 @@
       <c r="E228" t="s">
         <v>234</v>
       </c>
-      <c r="H228" s="5" t="str">
+      <c r="F228" s="7"/>
+      <c r="H228" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="225" Shortname="Frnlcht_vr" Duration="0" FunctionTypeCS2="Fernlicht_vorne_hinten" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6918,7 +7043,8 @@
       <c r="E229" t="s">
         <v>235</v>
       </c>
-      <c r="H229" s="5" t="str">
+      <c r="F229" s="7"/>
+      <c r="H229" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="226" Shortname="Strnlcht_v" Duration="0" FunctionTypeCS2="Stirnlicht_vorne_hinten" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6940,7 +7066,8 @@
       <c r="E230" t="s">
         <v>236</v>
       </c>
-      <c r="H230" s="5" t="str">
+      <c r="F230" s="7"/>
+      <c r="H230" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="227" Shortname="Lcht_Gnrtr" Duration="0" FunctionTypeCS2="Licht_Generator_Sound_hinten" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -6962,10 +7089,10 @@
       <c r="E231" t="s">
         <v>237</v>
       </c>
-      <c r="F231" t="s">
+      <c r="F231" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="H231" s="5" t="str">
+      <c r="H231" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="228" Shortname="Tlx_Wlzr_v" Duration="0" FunctionTypeCS2="Telex_Walzer_vorne" FunctionTypeZ21="decouple" /&gt;</v>
       </c>
@@ -6987,10 +7114,10 @@
       <c r="E232" t="s">
         <v>238</v>
       </c>
-      <c r="F232" t="s">
+      <c r="F232" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="H232" s="5" t="str">
+      <c r="H232" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="229" Shortname="Tlx_Wlzr_h" Duration="0" FunctionTypeCS2="Telex_Walzer_hinten" FunctionTypeZ21="decouple" /&gt;</v>
       </c>
@@ -7012,7 +7139,8 @@
       <c r="E233" t="s">
         <v>239</v>
       </c>
-      <c r="H233" s="5" t="str">
+      <c r="F233" s="7"/>
+      <c r="H233" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="230" Shortname="Lcht_Gnrtr" Duration="0" FunctionTypeCS2="Licht_Generator_Sound_vorne" FunctionTypeZ21="" /&gt;</v>
       </c>
@@ -7034,18 +7162,20 @@
       <c r="E234" t="s">
         <v>240</v>
       </c>
-      <c r="H234" s="5" t="str">
+      <c r="F234" s="7"/>
+      <c r="H234" s="8" t="str">
         <f t="shared" si="7"/>
         <v>&lt;mapping Id="231" Shortname="Krbln_Snd" Duration="0" FunctionTypeCS2="Kurbeln_Sound" FunctionTypeZ21="" /&gt;</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H235" s="5" t="s">
+      <c r="H235" s="8" t="s">
         <v>332</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:H234" xr:uid="{6998C7BB-3F10-8F46-AE0B-DDB5392E341E}"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" sort="0" autoFilter="0"/>
+  <autoFilter ref="A3:F3" xr:uid="{6998C7BB-3F10-8F46-AE0B-DDB5392E341E}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
@@ -7085,13 +7215,13 @@
       <c r="A1" t="s">
         <v>241</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">

</xml_diff>